<commit_message>
Adição de dados do baba 4 (T11B04)
</commit_message>
<xml_diff>
--- a/Teste_1_Jogador_Completo/Resultados_Ranking.xlsx
+++ b/Teste_1_Jogador_Completo/Resultados_Ranking.xlsx
@@ -10089,7 +10089,7 @@
         <v>0</v>
       </c>
       <c r="AB86" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC86" t="n">
         <v>0</v>
@@ -10107,10 +10107,10 @@
         <v>0</v>
       </c>
       <c r="AH86" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="AI86" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="87">
@@ -10538,7 +10538,7 @@
         <v>0</v>
       </c>
       <c r="AA90" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB90" t="n">
         <v>0</v>
@@ -10559,10 +10559,10 @@
         <v>0</v>
       </c>
       <c r="AH90" t="n">
+        <v>15</v>
+      </c>
+      <c r="AI90" t="n">
         <v>12</v>
-      </c>
-      <c r="AI90" t="n">
-        <v>9</v>
       </c>
     </row>
     <row r="91">
@@ -11207,7 +11207,7 @@
         <v>0</v>
       </c>
       <c r="X96" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y96" t="n">
         <v>0</v>
@@ -11237,10 +11237,10 @@
         <v>0</v>
       </c>
       <c r="AH96" t="n">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="AI96" t="n">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="97">
@@ -11338,7 +11338,7 @@
         <v>0</v>
       </c>
       <c r="AD97" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE97" t="n">
         <v>0</v>
@@ -11347,7 +11347,7 @@
         <v>0</v>
       </c>
       <c r="AG97" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH97" t="n">
         <v>30</v>
@@ -11573,7 +11573,7 @@
         <v>0</v>
       </c>
       <c r="AG99" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH99" t="n">
         <v>32</v>
@@ -11662,7 +11662,7 @@
         <v>0</v>
       </c>
       <c r="Y100" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z100" t="n">
         <v>0</v>
@@ -11900,7 +11900,7 @@
         <v>0</v>
       </c>
       <c r="AC102" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD102" t="n">
         <v>0</v>
@@ -11915,10 +11915,10 @@
         <v>0</v>
       </c>
       <c r="AH102" t="n">
+        <v>33</v>
+      </c>
+      <c r="AI102" t="n">
         <v>30</v>
-      </c>
-      <c r="AI102" t="n">
-        <v>27</v>
       </c>
     </row>
     <row r="103">
@@ -12882,7 +12882,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="C8" t="n">
         <v>11</v>
@@ -12951,7 +12951,7 @@
         <v>0</v>
       </c>
       <c r="Y8" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Z8" t="n">
         <v>0</v>
@@ -13067,7 +13067,7 @@
         <v>0</v>
       </c>
       <c r="AB9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC9" t="n">
         <v>0</v>
@@ -15204,10 +15204,10 @@
         <v>0</v>
       </c>
       <c r="AA29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC29" t="n">
         <v>1</v>
@@ -15557,7 +15557,7 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C33" t="n">
         <v>2</v>
@@ -15623,7 +15623,7 @@
         <v>0</v>
       </c>
       <c r="X33" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y33" t="n">
         <v>0</v>
@@ -15664,7 +15664,7 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C34" t="n">
         <v>7</v>
@@ -15736,7 +15736,7 @@
         <v>0</v>
       </c>
       <c r="Z34" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA34" t="n">
         <v>0</v>
@@ -15831,7 +15831,7 @@
         <v>0</v>
       </c>
       <c r="V35" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W35" t="n">
         <v>0</v>
@@ -15985,7 +15985,7 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C37" t="n">
         <v>17</v>
@@ -16042,7 +16042,7 @@
         <v>0</v>
       </c>
       <c r="U37" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V37" t="n">
         <v>0</v>
@@ -17047,7 +17047,7 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F5" t="n">
         <v>2</v>
@@ -17335,7 +17335,7 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="F14" t="n">
         <v>7</v>
@@ -17399,7 +17399,7 @@
         </is>
       </c>
       <c r="E16" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="F16" t="n">
         <v>1</v>
@@ -17431,7 +17431,7 @@
         </is>
       </c>
       <c r="E17" t="n">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F17" t="n">
         <v>5</v>

</xml_diff>